<commit_message>
feat: Adding the choose for extracting file or txt
</commit_message>
<xml_diff>
--- a/output/cardapio.xlsx
+++ b/output/cardapio.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -535,7 +535,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ling.Caseira</t>
+          <t>Linguiça Caseira</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -543,7 +543,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Asa</t>
+          <t>Asa de Frango</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -690,7 +690,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ling. mista</t>
+          <t>Linguiça Mista</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -752,7 +752,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Coração Galinha</t>
+          <t>Coração de Galinha</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -760,7 +760,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -845,7 +845,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Camarão alho e óleo</t>
+          <t>Cupim c/ Queijo</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -853,7 +853,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ESPETOS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -870,13 +870,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Cupim c/ queijo</t>
+          <t>Baião Enxuto P</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -884,7 +884,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -901,13 +901,13 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Carne sol c/macax</t>
+          <t>Baião Enxuto G</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -915,7 +915,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Espetos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -932,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Baião enxuto P</t>
+          <t>Baião Cremoso P</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -946,7 +946,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -963,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Baião enxuto G</t>
+          <t>Baião Cremoso G</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -977,7 +977,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -994,13 +994,13 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Baião Cremoso P</t>
+          <t>Arroz P</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1025,13 +1025,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Baião Cremoso G</t>
+          <t>Arroz G</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1056,13 +1056,13 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Arroz P</t>
+          <t>Macaxeira Frita</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1087,13 +1087,13 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Arroz G</t>
+          <t>Creme de Macaxeira</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1118,13 +1118,13 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Macaxeira frita</t>
+          <t>Batata Frita</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1149,13 +1149,13 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Creme de Macaxeira</t>
+          <t>Piabinha</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1180,13 +1180,13 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Batata frita</t>
+          <t>Torresmo</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1217,7 +1217,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Piabinha</t>
+          <t>Caldinho de Feijão</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1242,13 +1242,13 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Torresmo</t>
+          <t>Camarão c/ Alho e Óleo</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1273,13 +1273,13 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Caldinho de Feijão</t>
+          <t>Queijo na chapa</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1304,13 +1304,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Queijo na chapa</t>
+          <t>Carne de sol c/ Macaxeira</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Acompanhamentos</t>
+          <t>ACOMPANHAMENTOS</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Jantinhas</t>
+          <t>JANTINHAS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Jantinhas</t>
+          <t>JANTINHAS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Jantinhas</t>
+          <t>JANTINHAS</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Refri Lata</t>
+          <t>Porção Mungunzá mesa</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>MUNGUNZÁ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1521,13 +1521,13 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Refri 600</t>
+          <t>Porção Mungunzá viagem</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>MUNGUNZÁ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1552,13 +1552,13 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Refri 1L</t>
+          <t>Refri Lata</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1583,13 +1583,13 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Refri 1,5L</t>
+          <t>Refri 600ml</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1614,13 +1614,13 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Água</t>
+          <t>Refri 1L</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1645,13 +1645,13 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Água C/ gás</t>
+          <t>Refri 1,5L</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1676,13 +1676,13 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>3.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Cerveja buchuda</t>
+          <t>Água</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1707,13 +1707,13 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Long Neck</t>
+          <t>Água c/ gás</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1738,13 +1738,13 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Dose</t>
+          <t>Cerveja Buchuda</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1769,13 +1769,13 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Copo</t>
+          <t>Long Neck</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1800,13 +1800,13 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Suco S/L</t>
+          <t>Dose</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1831,13 +1831,13 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Suco C/L</t>
+          <t>Copo</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1845,7 +1845,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1862,13 +1862,13 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Cerveja 600ml</t>
+          <t>Suco S/L</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>bebidas</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1893,13 +1893,13 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Porção mesa</t>
+          <t>Suco C/L</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>sexta Do mungunzá</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1924,13 +1924,13 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Porção viagem</t>
+          <t>Cerveja 600ml</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1938,7 +1938,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>sexta Do mungunzá</t>
+          <t>BEBIDAS</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>